<commit_message>
Nerfs to Merchant Class Specialties
</commit_message>
<xml_diff>
--- a/resources/data-imports/Affixes/dodge.xlsx
+++ b/resources/data-imports/Affixes/dodge.xlsx
@@ -746,9 +746,6 @@
       <c r="U2">
         <v>0</v>
       </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
       <c r="X2">
         <v>10</v>
       </c>
@@ -803,7 +800,7 @@
         <v>45</v>
       </c>
       <c r="L3">
-        <v>0.0194</v>
+        <v>0.1</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -830,9 +827,6 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="W3">
         <v>0</v>
       </c>
       <c r="X3">
@@ -889,7 +883,7 @@
         <v>47</v>
       </c>
       <c r="L4">
-        <v>0.0376</v>
+        <v>0.2</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -916,9 +910,6 @@
         <v>0</v>
       </c>
       <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="W4">
         <v>0</v>
       </c>
       <c r="X4">
@@ -972,7 +963,7 @@
         <v>49</v>
       </c>
       <c r="L5">
-        <v>0.0729</v>
+        <v>0.29</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -999,9 +990,6 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="W5">
         <v>0</v>
       </c>
       <c r="X5">
@@ -1055,7 +1043,7 @@
         <v>51</v>
       </c>
       <c r="L6">
-        <v>0.1414</v>
+        <v>0.38</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1082,9 +1070,6 @@
         <v>0</v>
       </c>
       <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="W6">
         <v>0</v>
       </c>
       <c r="X6">
@@ -1138,7 +1123,7 @@
         <v>53</v>
       </c>
       <c r="L7">
-        <v>0.2885</v>
+        <v>0.47</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1165,9 +1150,6 @@
         <v>0</v>
       </c>
       <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="W7">
         <v>0</v>
       </c>
       <c r="X7">
@@ -1221,7 +1203,7 @@
         <v>55</v>
       </c>
       <c r="L8">
-        <v>0.5652</v>
+        <v>0.57</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1248,9 +1230,6 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="W8">
         <v>0</v>
       </c>
       <c r="X8">
@@ -1304,7 +1283,7 @@
         <v>57</v>
       </c>
       <c r="L9">
-        <v>0.88</v>
+        <v>0.66</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1331,9 +1310,6 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="W9">
         <v>0</v>
       </c>
       <c r="X9">
@@ -1387,7 +1363,7 @@
         <v>59</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1414,9 +1390,6 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="W10">
         <v>0</v>
       </c>
       <c r="X10">

</xml_diff>